<commit_message>
Add daily scrum, updated Burndown chart, mob programming pic
</commit_message>
<xml_diff>
--- a/admin/5-JulSprintBurndown.xlsx
+++ b/admin/5-JulSprintBurndown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elari\Documents\Repos\CSCI_S71\Teamify\admin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elari\floobits\share\mhaak\Teamify2020\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22237112-0238-4D25-94FA-A0A384E69E68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC37394C-FF4F-418A-8116-55989942C015}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21090" yWindow="-13995" windowWidth="18270" windowHeight="12315" xr2:uid="{E7DD3797-FEF2-40B3-90F6-28EA74433530}"/>
+    <workbookView xWindow="15870" yWindow="-13935" windowWidth="19875" windowHeight="12150" xr2:uid="{E7DD3797-FEF2-40B3-90F6-28EA74433530}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Teamify Project Progress</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Sprint</t>
   </si>
@@ -61,12 +58,33 @@
   <si>
     <t>Completed</t>
   </si>
+  <si>
+    <t>Velocity</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Teamify Sprint Performance</t>
+  </si>
+  <si>
+    <t>Goal</t>
+  </si>
+  <si>
+    <t>"Display resgistered students and team names"</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,6 +94,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -109,7 +136,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -117,19 +144,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -231,11 +280,99 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$5</c:f>
+              <c:f>Sheet1!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Expected</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$7:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>44013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44014</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44015</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44017</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44018</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$7:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3BD3-42CF-AC6E-40565FA7E075}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -258,10 +395,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$6:$A$10</c:f>
+              <c:f>Sheet1!$A$7:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>44013</c:v>
                 </c:pt>
@@ -276,29 +413,35 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>44017</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44018</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$B$10</c:f>
+              <c:f>Sheet1!$C$7:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -313,10 +456,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$5</c:f>
+              <c:f>Sheet1!$E$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -339,10 +482,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$6:$A$10</c:f>
+              <c:f>Sheet1!$A$7:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>44013</c:v>
                 </c:pt>
@@ -357,30 +500,36 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>44017</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44018</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$6:$D$10</c:f>
+              <c:f>Sheet1!$E$7:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -475,7 +624,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1153,16 +1302,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>455295</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>55245</xdr:rowOff>
+      <xdr:rowOff>150495</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1487,132 +1636,210 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA9E9F30-5C11-4B47-B69A-AD9990B127A1}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
+    <col min="2" max="2" width="10.68359375" customWidth="1"/>
     <col min="3" max="3" width="10.15625" customWidth="1"/>
     <col min="4" max="4" width="9.9453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="10">
+        <v>44018</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="11">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="3">
+        <v>44013</v>
+      </c>
+      <c r="B7" s="4">
+        <f>B4</f>
+        <v>10</v>
+      </c>
+      <c r="C7" s="5">
+        <v>10</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7">
+        <f>$B$4-SUM($D$7:D7)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="3">
+        <v>44014</v>
+      </c>
+      <c r="B8" s="4">
+        <f>B7-($B$4/ROWS($A$8:$A$12))</f>
+        <v>8</v>
+      </c>
+      <c r="C8" s="5">
+        <v>10</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7">
+        <f>$B$4-SUM($D$7:D8)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="3">
+        <v>44015</v>
+      </c>
+      <c r="B9" s="4">
+        <f t="shared" ref="B9:B12" si="0">B8-($B$4/ROWS($A$8:$A$12))</f>
+        <v>6</v>
+      </c>
+      <c r="C9" s="5">
+        <v>7</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1</v>
+      </c>
+      <c r="E9" s="7">
+        <f>$B$4-SUM($D$7:D9)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="3">
+        <v>44016</v>
+      </c>
+      <c r="B10" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C10" s="5">
+        <v>2</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="7">
+        <f>$B$4-SUM($D$7:D10)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="3">
         <v>44017</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
+      <c r="B11" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <f>$B$4-SUM($D$7:D11)</f>
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="3">
+        <v>44018</v>
+      </c>
+      <c r="B12" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="7">
+        <f>$B$4-SUM($D$7:D12)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="8">
+        <f>B7-B12</f>
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="3">
-        <v>44013</v>
-      </c>
-      <c r="B6" s="7">
+      <c r="C14" s="8">
+        <f>C7-C12</f>
         <v>10</v>
       </c>
-      <c r="C6" s="5">
-        <v>0</v>
-      </c>
-      <c r="D6" s="6">
-        <f>$B$3-SUM($C$6:C6)</f>
+      <c r="D14" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="3">
-        <v>44014</v>
-      </c>
-      <c r="B7" s="7">
-        <v>8</v>
-      </c>
-      <c r="C7" s="5">
-        <v>3</v>
-      </c>
-      <c r="D7" s="6">
-        <f>$B$3-SUM($C$6:C7)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="3">
-        <v>44015</v>
-      </c>
-      <c r="B8" s="7">
-        <v>6</v>
-      </c>
-      <c r="C8" s="5">
-        <v>4</v>
-      </c>
-      <c r="D8" s="6">
-        <f>$B$3-SUM($C$6:C8)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="3">
-        <v>44016</v>
-      </c>
-      <c r="B9" s="7">
-        <v>3</v>
-      </c>
-      <c r="C9" s="5">
-        <v>2</v>
-      </c>
-      <c r="D9" s="6">
-        <f>$B$3-SUM($C$6:C9)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="3">
-        <v>44017</v>
-      </c>
-      <c r="B10" s="7">
-        <v>0</v>
-      </c>
-      <c r="C10" s="5">
-        <v>0</v>
-      </c>
-      <c r="D10" s="6">
-        <f>$B$3-SUM($C$6:C10)</f>
+      <c r="E14" s="2">
+        <f t="shared" ref="E14" si="1">E7-E12</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>